<commit_message>
Pesan commit yang menjelaskan perubahan
</commit_message>
<xml_diff>
--- a/src/query/tes_mentor.xlsx
+++ b/src/query/tes_mentor.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>ID Mentor</t>
   </si>
@@ -32,10 +32,13 @@
     <t>tes</t>
   </si>
   <si>
-    <t>tes@tes</t>
+    <t>tes@te</t>
   </si>
   <si>
     <t>nurma</t>
+  </si>
+  <si>
+    <t>apapun@telkom.co.id</t>
   </si>
   <si>
     <t>sleman</t>
@@ -430,8 +433,11 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -439,13 +445,13 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>